<commit_message>
Modificando el diseño estructuras
</commit_message>
<xml_diff>
--- a/disenioEstructurasJanMerinoFabersani.xlsx
+++ b/disenioEstructurasJanMerinoFabersani.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="89">
   <si>
     <t xml:space="preserve">DISEÑO DE ESTRUCTURAS DE DATOS:</t>
   </si>
@@ -199,13 +199,10 @@
     <t xml:space="preserve">ESTADO_LETRA_DISPONIBLE</t>
   </si>
   <si>
-    <t xml:space="preserve">Tipo:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tipos de datos:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">¿Para qué se utiliza?:</t>
+    <t xml:space="preserve">Tipo: Asociativo(Las claves son letras alfabetícas )</t>
+  </si>
+  <si>
+    <t xml:space="preserve">¿Para qué se utiliza?: Se utiliza para guardar el estado de una letra</t>
   </si>
   <si>
     <t xml:space="preserve">$ordenTeclado =</t>
@@ -214,168 +211,54 @@
     <t xml:space="preserve">salto</t>
   </si>
   <si>
+    <t xml:space="preserve">¿Para qué se utiliza?: Se utiliza para mostrar el orden en que se debe escribir el teclado en pantalla</t>
+  </si>
+  <si>
     <t xml:space="preserve">$estructuraIntentosWordix =</t>
   </si>
   <si>
     <t xml:space="preserve">//Mas indices…</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">[“letra” =&gt; “q”, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">“estado” =&gt; “descartada”]</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">[“letra” =&gt; “f”, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">“estado” =&gt; “descartada”]</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">[“letra” =&gt; “u”, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">“estado” =&gt; “descartada”]</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">[“letra” =&gt; “e”, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">“estado” =&gt; “descartada”]</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">[“letra” =&gt; “s”, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">“estado” =&gt; “descartada”]</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">[“letra” =&gt; “g”, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">“estado” =&gt; “descartada”]</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">[“letra” =&gt; “o”, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">“estado” =&gt; “descartada”]</t>
-    </r>
+    <t xml:space="preserve">[“letra” =&gt; “q”, “estado” =&gt; “descartada”]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[“letra” =&gt; “f”, “estado” =&gt; “descartada”]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[“letra” =&gt; “u”, “estado” =&gt; “descartada”]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[“letra” =&gt; “e”, “estado” =&gt; “descartada”]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[“letra” =&gt; “s”, “estado” =&gt; “descartada”]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[“letra” =&gt; “g”, “estado” =&gt; “descartada”]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[“letra” =&gt; “o”, “estado” =&gt; “descartada”]</t>
   </si>
   <si>
     <t xml:space="preserve">//Mas valores…</t>
   </si>
   <si>
-    <t xml:space="preserve">Tipo: </t>
+    <t xml:space="preserve">Tipo: multidimensional (Indices numericos y claves string)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">¿Para qué se utiliza?: Se utiliza para guardar los intentos de Wordix para adivinar la palabra</t>
   </si>
   <si>
     <t xml:space="preserve">$estructuraPalabraIntento =</t>
   </si>
   <si>
+    <t xml:space="preserve">Tipo: multidimensional(Indices numericos y claves string)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">¿Para qué se utiliza?: Se utiliza para guardar el intento actual</t>
+  </si>
+  <si>
     <t xml:space="preserve">$partida =</t>
   </si>
   <si>
@@ -395,6 +278,15 @@
   </si>
   <si>
     <t xml:space="preserve">“pepito”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tipo: Asociativo(Las claves son string )</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tipos de datos: Almacena valores String y enteros</t>
+  </si>
+  <si>
+    <t xml:space="preserve">¿Para qué se utiliza?: SE utiliza para información de la partida</t>
   </si>
 </sst>
 </file>
@@ -404,7 +296,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -458,12 +350,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -652,10 +538,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AE70"/>
+  <dimension ref="A1:AE66"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="77" zoomScaleNormal="77" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G65" activeCellId="0" sqref="G65"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="88" zoomScaleNormal="88" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F68" activeCellId="0" sqref="F68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -667,8 +553,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="12.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="13.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="13.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="12.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="12.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="12.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="12.71"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1021,19 +907,19 @@
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="1" t="s">
-        <v>60</v>
+        <v>26</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B21" s="3" t="n">
         <v>0</v>
@@ -1128,7 +1014,7 @@
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C22" s="8" t="s">
         <v>46</v>
@@ -1161,7 +1047,7 @@
         <v>45</v>
       </c>
       <c r="M22" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="N22" s="8" t="s">
         <v>29</v>
@@ -1191,7 +1077,7 @@
         <v>40</v>
       </c>
       <c r="W22" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="X22" s="8" t="s">
         <v>55</v>
@@ -1226,24 +1112,21 @@
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="1" t="s">
-        <v>59</v>
+        <v>25</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="1" t="s">
-        <v>60</v>
+        <v>26</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="12" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="0"/>
-    </row>
-    <row r="30" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="10" t="s">
         <v>64</v>
       </c>
@@ -1253,9 +1136,6 @@
       <c r="C30" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D30" s="0"/>
-      <c r="E30" s="0"/>
-      <c r="F30" s="0"/>
       <c r="G30" s="3" t="n">
         <v>1</v>
       </c>
@@ -1273,8 +1153,6 @@
       <c r="B31" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C31" s="0"/>
-      <c r="D31" s="0"/>
       <c r="E31" s="9" t="s">
         <v>23</v>
       </c>
@@ -1295,8 +1173,6 @@
       <c r="B32" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C32" s="0"/>
-      <c r="D32" s="0"/>
       <c r="E32" s="9" t="s">
         <v>23</v>
       </c>
@@ -1317,8 +1193,6 @@
       <c r="B33" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="C33" s="0"/>
-      <c r="D33" s="0"/>
       <c r="E33" s="9" t="s">
         <v>23</v>
       </c>
@@ -1339,8 +1213,6 @@
       <c r="B34" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C34" s="0"/>
-      <c r="D34" s="0"/>
       <c r="E34" s="9" t="s">
         <v>23</v>
       </c>
@@ -1361,8 +1233,6 @@
       <c r="B35" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C35" s="0"/>
-      <c r="D35" s="0"/>
       <c r="E35" s="9" t="s">
         <v>23</v>
       </c>
@@ -1383,9 +1253,6 @@
       <c r="B36" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="C36" s="0"/>
-      <c r="D36" s="0"/>
-      <c r="E36" s="0"/>
       <c r="F36" s="6" t="s">
         <v>2</v>
       </c>
@@ -1397,69 +1264,34 @@
       <c r="A37" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="B37" s="0"/>
-      <c r="C37" s="0"/>
-      <c r="D37" s="0"/>
-      <c r="E37" s="0"/>
       <c r="F37" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="G37" s="0"/>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0"/>
       <c r="B38" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C38" s="0"/>
-      <c r="D38" s="0"/>
-      <c r="E38" s="0"/>
-      <c r="F38" s="0"/>
-      <c r="G38" s="0"/>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0"/>
       <c r="B39" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C39" s="0"/>
-      <c r="D39" s="0"/>
-      <c r="E39" s="0"/>
-      <c r="F39" s="0"/>
-      <c r="G39" s="0"/>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="0"/>
       <c r="B40" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="C40" s="0"/>
-      <c r="D40" s="0"/>
-      <c r="E40" s="0"/>
-      <c r="F40" s="0"/>
-      <c r="G40" s="0"/>
+        <v>26</v>
+      </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B41" s="12" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B43" s="0"/>
-    </row>
-    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B44" s="0"/>
+        <v>75</v>
+      </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="B45" s="0"/>
-      <c r="C45" s="0"/>
-      <c r="D45" s="0"/>
-      <c r="E45" s="0"/>
-      <c r="F45" s="0"/>
-      <c r="G45" s="0"/>
+        <v>76</v>
+      </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="3" t="n">
@@ -1468,13 +1300,9 @@
       <c r="B46" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C46" s="0"/>
-      <c r="D46" s="0"/>
       <c r="E46" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="F46" s="0"/>
-      <c r="G46" s="0"/>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="5" t="n">
@@ -1483,13 +1311,9 @@
       <c r="B47" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C47" s="0"/>
-      <c r="D47" s="0"/>
       <c r="E47" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="F47" s="0"/>
-      <c r="G47" s="0"/>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="5" t="n">
@@ -1498,12 +1322,9 @@
       <c r="B48" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="C48" s="0"/>
-      <c r="D48" s="0"/>
       <c r="E48" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="F48" s="0"/>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="5" t="n">
@@ -1512,12 +1333,9 @@
       <c r="B49" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C49" s="0"/>
-      <c r="D49" s="0"/>
       <c r="E49" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="F49" s="0"/>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="5" t="n">
@@ -1526,93 +1344,50 @@
       <c r="B50" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C50" s="0"/>
-      <c r="D50" s="0"/>
       <c r="E50" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="F50" s="0"/>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B51" s="0"/>
-      <c r="C51" s="0"/>
-      <c r="D51" s="0"/>
-      <c r="E51" s="0"/>
-      <c r="F51" s="0"/>
-    </row>
-    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="0"/>
-      <c r="B52" s="0"/>
-      <c r="C52" s="0"/>
-      <c r="D52" s="0"/>
-      <c r="E52" s="0"/>
-      <c r="F52" s="0"/>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="0"/>
       <c r="B53" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C53" s="0"/>
-      <c r="D53" s="0"/>
-      <c r="E53" s="0"/>
-      <c r="F53" s="0"/>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="0"/>
-      <c r="B54" s="1" t="s">
-        <v>59</v>
+      <c r="B54" s="12" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B55" s="1" t="s">
-        <v>60</v>
+        <v>26</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="0"/>
       <c r="B56" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="C56" s="0"/>
-      <c r="D56" s="0"/>
-      <c r="E56" s="0"/>
-      <c r="F56" s="0"/>
-    </row>
-    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="0"/>
-      <c r="B57" s="0"/>
-      <c r="C57" s="0"/>
-      <c r="D57" s="0"/>
-      <c r="E57" s="0"/>
-      <c r="F57" s="0"/>
-    </row>
-    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="0"/>
-      <c r="B58" s="0"/>
-      <c r="C58" s="0"/>
-      <c r="D58" s="0"/>
-      <c r="E58" s="0"/>
-      <c r="F58" s="0"/>
+        <v>78</v>
+      </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="10" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="B59" s="8" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="C59" s="8" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="D59" s="8" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="E59" s="8" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="F59" s="6" t="s">
         <v>56</v>
@@ -1620,10 +1395,10 @@
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B60" s="8" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="C60" s="8" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="D60" s="8" t="n">
         <v>1</v>
@@ -1642,54 +1417,18 @@
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B64" s="1" t="s">
-        <v>59</v>
+        <v>86</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B65" s="1" t="s">
-        <v>60</v>
+        <v>87</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B66" s="12" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="0"/>
-      <c r="B67" s="0"/>
-      <c r="C67" s="0"/>
-      <c r="D67" s="0"/>
-      <c r="E67" s="0"/>
-      <c r="F67" s="0"/>
-      <c r="G67" s="0"/>
-    </row>
-    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="0"/>
-      <c r="B68" s="0"/>
-      <c r="C68" s="0"/>
-      <c r="D68" s="0"/>
-      <c r="E68" s="0"/>
-      <c r="F68" s="0"/>
-      <c r="G68" s="0"/>
-    </row>
-    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="0"/>
-      <c r="B69" s="0"/>
-      <c r="C69" s="0"/>
-      <c r="D69" s="0"/>
-      <c r="E69" s="0"/>
-      <c r="F69" s="0"/>
-      <c r="G69" s="0"/>
-    </row>
-    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="0"/>
-      <c r="B70" s="0"/>
-      <c r="C70" s="0"/>
-      <c r="D70" s="0"/>
-      <c r="E70" s="0"/>
-      <c r="F70" s="0"/>
-      <c r="G70" s="0"/>
+        <v>88</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Se modifica las funciones partidaGanada y estadisticasJugador, ademas se agrega una array asociativa en la funcion estadisticasDeJugador.
</commit_message>
<xml_diff>
--- a/disenioEstructurasJanMerinoFabersani.xlsx
+++ b/disenioEstructurasJanMerinoFabersani.xlsx
@@ -1,16 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\clona\OneDrive\Documents\tp final\Wordix-grupo-10\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{318FB02A-4D48-4A4E-886E-F02EB3D84C6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="EstructuraDatos" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="EstructuraDatos" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -20,325 +25,394 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="103">
-  <si>
-    <t xml:space="preserve">DISEÑO DE ESTRUCTURAS DE DATOS:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">$coleccionPalabras =</t>
-  </si>
-  <si>
-    <t xml:space="preserve">//indices</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MUJER</t>
-  </si>
-  <si>
-    <t xml:space="preserve">QUESO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FUEGO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CASAS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RASGO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GATOS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GOTAS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HUEVO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TINTO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NAVES</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VERDE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MELON</t>
-  </si>
-  <si>
-    <t xml:space="preserve">YUYOS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PIANO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PISOS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JAMON</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ROSAS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VACAS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MOVIL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ANIME</t>
-  </si>
-  <si>
-    <t xml:space="preserve">//valores</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Información de la estructura:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tipo: Indexado (los índices son numéricos)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tipos de datos: Almacena valores String</t>
-  </si>
-  <si>
-    <t xml:space="preserve">¿Para qué se utiliza?: guarda las palabras que se pueden elegir para jugar Wordix</t>
-  </si>
-  <si>
-    <t xml:space="preserve">$teclado =</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E</t>
-  </si>
-  <si>
-    <t xml:space="preserve">F</t>
-  </si>
-  <si>
-    <t xml:space="preserve">G</t>
-  </si>
-  <si>
-    <t xml:space="preserve">H</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I</t>
-  </si>
-  <si>
-    <t xml:space="preserve">J</t>
-  </si>
-  <si>
-    <t xml:space="preserve">K</t>
-  </si>
-  <si>
-    <t xml:space="preserve">L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M</t>
-  </si>
-  <si>
-    <t xml:space="preserve">N</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ñ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">O</t>
-  </si>
-  <si>
-    <t xml:space="preserve">P</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Q</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R</t>
-  </si>
-  <si>
-    <t xml:space="preserve">S</t>
-  </si>
-  <si>
-    <t xml:space="preserve">T</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U</t>
-  </si>
-  <si>
-    <t xml:space="preserve">V</t>
-  </si>
-  <si>
-    <t xml:space="preserve">W</t>
-  </si>
-  <si>
-    <t xml:space="preserve">X</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Y</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Z</t>
-  </si>
-  <si>
-    <t xml:space="preserve">//claves</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="127">
+  <si>
+    <t>DISEÑO DE ESTRUCTURAS DE DATOS:</t>
+  </si>
+  <si>
+    <t>$coleccionPalabras =</t>
+  </si>
+  <si>
+    <t>//indices</t>
+  </si>
+  <si>
+    <t>MUJER</t>
+  </si>
+  <si>
+    <t>QUESO</t>
+  </si>
+  <si>
+    <t>FUEGO</t>
+  </si>
+  <si>
+    <t>CASAS</t>
+  </si>
+  <si>
+    <t>RASGO</t>
+  </si>
+  <si>
+    <t>GATOS</t>
+  </si>
+  <si>
+    <t>GOTAS</t>
+  </si>
+  <si>
+    <t>HUEVO</t>
+  </si>
+  <si>
+    <t>TINTO</t>
+  </si>
+  <si>
+    <t>NAVES</t>
+  </si>
+  <si>
+    <t>VERDE</t>
+  </si>
+  <si>
+    <t>MELON</t>
+  </si>
+  <si>
+    <t>YUYOS</t>
+  </si>
+  <si>
+    <t>PIANO</t>
+  </si>
+  <si>
+    <t>PISOS</t>
+  </si>
+  <si>
+    <t>JAMON</t>
+  </si>
+  <si>
+    <t>ROSAS</t>
+  </si>
+  <si>
+    <t>VACAS</t>
+  </si>
+  <si>
+    <t>MOVIL</t>
+  </si>
+  <si>
+    <t>ANIME</t>
+  </si>
+  <si>
+    <t>//valores</t>
+  </si>
+  <si>
+    <t>Información de la estructura:</t>
+  </si>
+  <si>
+    <t>Tipo: Indexado (los índices son numéricos)</t>
+  </si>
+  <si>
+    <t>Tipos de datos: Almacena valores String</t>
+  </si>
+  <si>
+    <t>¿Para qué se utiliza?: guarda las palabras que se pueden elegir para jugar Wordix</t>
+  </si>
+  <si>
+    <t>$teclado =</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>J</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>Ñ</t>
+  </si>
+  <si>
+    <t>O</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>Q</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>Z</t>
+  </si>
+  <si>
+    <t>//claves</t>
   </si>
   <si>
     <t xml:space="preserve">ESTADO_LETRA_DISPONIBLE </t>
   </si>
   <si>
-    <t xml:space="preserve">ESTADO_LETRA_DISPONIBLE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tipo: Asociativo(Las claves son letras alfabetícas )</t>
-  </si>
-  <si>
-    <t xml:space="preserve">¿Para qué se utiliza?: Se utiliza para guardar el estado de una letra</t>
-  </si>
-  <si>
-    <t xml:space="preserve">$ordenTeclado =</t>
-  </si>
-  <si>
-    <t xml:space="preserve">salto</t>
-  </si>
-  <si>
-    <t xml:space="preserve">¿Para qué se utiliza?: Se utiliza para mostrar el orden en que se debe escribir el teclado en pantalla</t>
-  </si>
-  <si>
-    <t xml:space="preserve">$estructuraIntentosWordix =</t>
-  </si>
-  <si>
-    <t xml:space="preserve">//Mas indices…</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[“letra” =&gt; “q”, “estado” =&gt; “descartada”]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[“letra” =&gt; “f”, “estado” =&gt; “descartada”]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[“letra” =&gt; “u”, “estado” =&gt; “descartada”]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[“letra” =&gt; “e”, “estado” =&gt; “descartada”]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[“letra” =&gt; “s”, “estado” =&gt; “descartada”]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[“letra” =&gt; “g”, “estado” =&gt; “descartada”]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[“letra” =&gt; “o”, “estado” =&gt; “descartada”]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">//Mas valores…</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tipo: multidimensional (Indices numericos y claves string)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">¿Para qué se utiliza?: Se utiliza para guardar los intentos de Wordix para adivinar la palabra</t>
-  </si>
-  <si>
-    <t xml:space="preserve">$estructuraPalabraIntento =</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tipo: multidimensional(Indices numericos y claves string)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">¿Para qué se utiliza?: Se utiliza para guardar el intento actual</t>
-  </si>
-  <si>
-    <t xml:space="preserve">$partida =</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"palabraWordix"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"jugador"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"intentos"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"puntaje"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">“fuego”</t>
-  </si>
-  <si>
-    <t xml:space="preserve">“pepito”</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tipo: Asociativo(Las claves son string )</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tipos de datos: Almacena valores String y enteros</t>
-  </si>
-  <si>
-    <t xml:space="preserve">¿Para qué se utiliza?: SE utiliza para información de la partida</t>
+    <t>ESTADO_LETRA_DISPONIBLE</t>
+  </si>
+  <si>
+    <t>Tipo: Asociativo(Las claves son letras alfabetícas )</t>
+  </si>
+  <si>
+    <t>¿Para qué se utiliza?: Se utiliza para guardar el estado de una letra</t>
+  </si>
+  <si>
+    <t>$ordenTeclado =</t>
+  </si>
+  <si>
+    <t>salto</t>
+  </si>
+  <si>
+    <t>¿Para qué se utiliza?: Se utiliza para mostrar el orden en que se debe escribir el teclado en pantalla</t>
+  </si>
+  <si>
+    <t>$estructuraIntentosWordix =</t>
+  </si>
+  <si>
+    <t>//Mas indices…</t>
+  </si>
+  <si>
+    <t>[“letra” =&gt; “q”, “estado” =&gt; “descartada”]</t>
+  </si>
+  <si>
+    <t>[“letra” =&gt; “f”, “estado” =&gt; “descartada”]</t>
+  </si>
+  <si>
+    <t>[“letra” =&gt; “u”, “estado” =&gt; “descartada”]</t>
+  </si>
+  <si>
+    <t>[“letra” =&gt; “e”, “estado” =&gt; “descartada”]</t>
+  </si>
+  <si>
+    <t>[“letra” =&gt; “s”, “estado” =&gt; “descartada”]</t>
+  </si>
+  <si>
+    <t>[“letra” =&gt; “g”, “estado” =&gt; “descartada”]</t>
+  </si>
+  <si>
+    <t>[“letra” =&gt; “o”, “estado” =&gt; “descartada”]</t>
+  </si>
+  <si>
+    <t>//Mas valores…</t>
+  </si>
+  <si>
+    <t>Tipo: multidimensional (Indices numericos y claves string)</t>
+  </si>
+  <si>
+    <t>¿Para qué se utiliza?: Se utiliza para guardar los intentos de Wordix para adivinar la palabra</t>
+  </si>
+  <si>
+    <t>$estructuraPalabraIntento =</t>
+  </si>
+  <si>
+    <t>Tipo: multidimensional(Indices numericos y claves string)</t>
+  </si>
+  <si>
+    <t>¿Para qué se utiliza?: Se utiliza para guardar el intento actual</t>
+  </si>
+  <si>
+    <t>$partida =</t>
+  </si>
+  <si>
+    <t>"palabraWordix"</t>
+  </si>
+  <si>
+    <t>"jugador"</t>
+  </si>
+  <si>
+    <t>"intentos"</t>
+  </si>
+  <si>
+    <t>"puntaje"</t>
+  </si>
+  <si>
+    <t>“fuego”</t>
+  </si>
+  <si>
+    <t>“pepito”</t>
+  </si>
+  <si>
+    <t>Tipo: Asociativo(Las claves son string )</t>
+  </si>
+  <si>
+    <t>Tipos de datos: Almacena valores String y enteros</t>
+  </si>
+  <si>
+    <t>¿Para qué se utiliza?: SE utiliza para información de la partida</t>
   </si>
   <si>
     <t xml:space="preserve">$coleccionPartidas = </t>
   </si>
   <si>
-    <t xml:space="preserve">["palabrawordix"=&gt;"vacas", "jugador"=&gt;"mari", "intentos"=&gt; 6 , "puntaje"=&gt; 0 ]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">["palabrawordix"=&gt;"mujer", "jugador"=&gt;"marian", "intentos"=&gt; 4 , "puntaje"=&gt; 12 ]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">["palabrawordix"=&gt;"gatos", "jugador"=&gt;"maria", "intentos"=&gt; 5 , "puntaje"=&gt; 12 ]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">["palabrawordix"=&gt;"gotas", "jugador"=&gt;"jose", "intentos"=&gt; 2 , "puntaje"=&gt; 15 ]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">["palabrawordix"=&gt;"huevo", "jugador"=&gt;"juan", "intentos"=&gt; 4 , "puntaje"=&gt; 11 ]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">["palabrawordix"=&gt;"queso", "jugador"=&gt;"manu", "intentos"=&gt; 3 , "puntaje"=&gt; 13 ]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">["palabrawordix"=&gt;"fuego", "jugador"=&gt;"pablo", "intentos"=&gt; 5 , "puntaje"=&gt; 9 ]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">["palabrawordix"=&gt;"casas", "jugador"=&gt;"santos", "intentos"=&gt; 3 , "puntaje"=&gt; 14 ]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">["palabrawordix"=&gt;"tinto", "jugador"=&gt;"manu", "intentos"=&gt; 1 , "puntaje"=&gt; 17 ]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">["palabrawordix"=&gt;"piano", "jugador"=&gt;"nisman", "intentos"=&gt; 2 , "puntaje"=&gt; 14 ]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">["palabrawordix"=&gt;"pisos", "jugador"=&gt;"nisman", "intentos"=&gt; 4 , "puntaje"=&gt; 14 ]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">["palabrawordix"=&gt;"verde", "jugador"=&gt;"marti", "intentos"=&gt; 3 , "puntaje"=&gt; 14 ]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">¿Para qué se utiliza?: Se utiliza para guardar información de las partidas</t>
+    <t>["palabrawordix"=&gt;"vacas", "jugador"=&gt;"mari", "intentos"=&gt; 6 , "puntaje"=&gt; 0 ]</t>
+  </si>
+  <si>
+    <t>["palabrawordix"=&gt;"mujer", "jugador"=&gt;"marian", "intentos"=&gt; 4 , "puntaje"=&gt; 12 ]</t>
+  </si>
+  <si>
+    <t>["palabrawordix"=&gt;"gatos", "jugador"=&gt;"maria", "intentos"=&gt; 5 , "puntaje"=&gt; 12 ]</t>
+  </si>
+  <si>
+    <t>["palabrawordix"=&gt;"gotas", "jugador"=&gt;"jose", "intentos"=&gt; 2 , "puntaje"=&gt; 15 ]</t>
+  </si>
+  <si>
+    <t>["palabrawordix"=&gt;"huevo", "jugador"=&gt;"juan", "intentos"=&gt; 4 , "puntaje"=&gt; 11 ]</t>
+  </si>
+  <si>
+    <t>["palabrawordix"=&gt;"queso", "jugador"=&gt;"manu", "intentos"=&gt; 3 , "puntaje"=&gt; 13 ]</t>
+  </si>
+  <si>
+    <t>["palabrawordix"=&gt;"fuego", "jugador"=&gt;"pablo", "intentos"=&gt; 5 , "puntaje"=&gt; 9 ]</t>
+  </si>
+  <si>
+    <t>["palabrawordix"=&gt;"casas", "jugador"=&gt;"santos", "intentos"=&gt; 3 , "puntaje"=&gt; 14 ]</t>
+  </si>
+  <si>
+    <t>["palabrawordix"=&gt;"tinto", "jugador"=&gt;"manu", "intentos"=&gt; 1 , "puntaje"=&gt; 17 ]</t>
+  </si>
+  <si>
+    <t>["palabrawordix"=&gt;"piano", "jugador"=&gt;"nisman", "intentos"=&gt; 2 , "puntaje"=&gt; 14 ]</t>
+  </si>
+  <si>
+    <t>["palabrawordix"=&gt;"pisos", "jugador"=&gt;"nisman", "intentos"=&gt; 4 , "puntaje"=&gt; 14 ]</t>
+  </si>
+  <si>
+    <t>["palabrawordix"=&gt;"verde", "jugador"=&gt;"marti", "intentos"=&gt; 3 , "puntaje"=&gt; 14 ]</t>
+  </si>
+  <si>
+    <t>¿Para qué se utiliza?: Se utiliza para guardar información de las partidas</t>
+  </si>
+  <si>
+    <t>       </t>
+  </si>
+  <si>
+    <t>$datosJugador=</t>
+  </si>
+  <si>
+    <t>$nombreJugador</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "jugador"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "partida"  </t>
+  </si>
+  <si>
+    <t>$partidasTotales</t>
+  </si>
+  <si>
+    <t>$puntajesTotales</t>
+  </si>
+  <si>
+    <t>$victoriasTotales</t>
+  </si>
+  <si>
+    <t>$intento1</t>
+  </si>
+  <si>
+    <t>$intento2</t>
+  </si>
+  <si>
+    <t>$intento3</t>
+  </si>
+  <si>
+    <t>$intento4</t>
+  </si>
+  <si>
+    <t>$intento5</t>
+  </si>
+  <si>
+    <t>$intento6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"puntaje" </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"victorias" </t>
+  </si>
+  <si>
+    <t>"intento1"</t>
+  </si>
+  <si>
+    <t>"intento2"</t>
+  </si>
+  <si>
+    <t>"intento3"</t>
+  </si>
+  <si>
+    <t>"intento4"</t>
+  </si>
+  <si>
+    <t>"intento5"</t>
+  </si>
+  <si>
+    <t>"intento6"</t>
+  </si>
+  <si>
+    <t>Tipo: asociativa ( claves string)</t>
+  </si>
+  <si>
+    <t>¿Para qué se utiliza?: Se utiliza para guardar información del resumen del jugador</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="General"/>
-  </numFmts>
-  <fonts count="9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -347,22 +421,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
+      <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -370,7 +429,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="11"/>
       <color rgb="FF808080"/>
       <name val="Calibri"/>
@@ -378,7 +437,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="10"/>
       <color rgb="FF808080"/>
       <name val="Calibri"/>
@@ -386,7 +445,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <i val="true"/>
+      <i/>
       <sz val="10"/>
       <color rgb="FF00B050"/>
       <name val="Calibri"/>
@@ -396,6 +455,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FF808080"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -410,119 +475,84 @@
     </fill>
   </fills>
   <borders count="3">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="14">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -581,110 +611,416 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:AE87"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AE95"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A58" colorId="64" zoomScale="88" zoomScaleNormal="88" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A69" activeCellId="0" sqref="A69:G81"/>
+    <sheetView tabSelected="1" topLeftCell="A76" zoomScale="88" zoomScaleNormal="88" workbookViewId="0">
+      <selection activeCell="F96" sqref="F96"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="25.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="14.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="13.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="13.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="12.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="13.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="13.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="12.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="12.71"/>
+    <col min="1" max="1" width="25.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" style="1" customWidth="1"/>
+    <col min="3" max="4" width="16.140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="14" style="1" customWidth="1"/>
+    <col min="8" max="8" width="12.85546875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="12.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="3" t="n">
+      <c r="B3" s="3">
         <v>0</v>
       </c>
-      <c r="C3" s="3" t="n">
+      <c r="C3" s="3">
         <v>1</v>
       </c>
-      <c r="D3" s="3" t="n">
+      <c r="D3" s="3">
         <v>2</v>
       </c>
-      <c r="E3" s="3" t="n">
+      <c r="E3" s="3">
         <v>3</v>
       </c>
-      <c r="F3" s="3" t="n">
+      <c r="F3" s="3">
         <v>4</v>
       </c>
-      <c r="G3" s="3" t="n">
+      <c r="G3" s="3">
         <v>5</v>
       </c>
-      <c r="H3" s="4" t="n">
+      <c r="H3" s="4">
         <v>6</v>
       </c>
-      <c r="I3" s="5" t="n">
+      <c r="I3" s="5">
         <v>7</v>
       </c>
-      <c r="J3" s="5" t="n">
+      <c r="J3" s="5">
         <v>8</v>
       </c>
-      <c r="K3" s="5" t="n">
+      <c r="K3" s="5">
         <v>9</v>
       </c>
-      <c r="L3" s="5" t="n">
+      <c r="L3" s="5">
         <v>10</v>
       </c>
-      <c r="M3" s="5" t="n">
+      <c r="M3" s="5">
         <v>11</v>
       </c>
-      <c r="N3" s="5" t="n">
+      <c r="N3" s="5">
         <v>12</v>
       </c>
-      <c r="O3" s="5" t="n">
+      <c r="O3" s="5">
         <v>13</v>
       </c>
-      <c r="P3" s="5" t="n">
+      <c r="P3" s="5">
         <v>14</v>
       </c>
-      <c r="Q3" s="5" t="n">
+      <c r="Q3" s="5">
         <v>15</v>
       </c>
-      <c r="R3" s="5" t="n">
+      <c r="R3" s="5">
         <v>16</v>
       </c>
-      <c r="S3" s="5" t="n">
+      <c r="S3" s="5">
         <v>17</v>
       </c>
-      <c r="T3" s="5" t="n">
+      <c r="T3" s="5">
         <v>18</v>
       </c>
-      <c r="U3" s="5" t="n">
+      <c r="U3" s="5">
         <v>19</v>
       </c>
       <c r="V3" s="6" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B4" s="7" t="s">
         <v>3</v>
       </c>
@@ -749,30 +1085,27 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>28</v>
       </c>
@@ -861,7 +1194,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="36.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:29" ht="45" x14ac:dyDescent="0.25">
       <c r="B13" s="11" t="s">
         <v>57</v>
       </c>
@@ -947,125 +1280,122 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B16" s="12" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B18" s="12" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A21" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="B21" s="3" t="n">
+      <c r="B21" s="3">
         <v>0</v>
       </c>
-      <c r="C21" s="3" t="n">
+      <c r="C21" s="3">
         <v>1</v>
       </c>
-      <c r="D21" s="3" t="n">
+      <c r="D21" s="3">
         <v>2</v>
       </c>
-      <c r="E21" s="3" t="n">
+      <c r="E21" s="3">
         <v>3</v>
       </c>
-      <c r="F21" s="3" t="n">
+      <c r="F21" s="3">
         <v>4</v>
       </c>
-      <c r="G21" s="3" t="n">
+      <c r="G21" s="3">
         <v>5</v>
       </c>
-      <c r="H21" s="4" t="n">
+      <c r="H21" s="4">
         <v>6</v>
       </c>
-      <c r="I21" s="5" t="n">
+      <c r="I21" s="5">
         <v>7</v>
       </c>
-      <c r="J21" s="5" t="n">
+      <c r="J21" s="5">
         <v>8</v>
       </c>
-      <c r="K21" s="5" t="n">
+      <c r="K21" s="5">
         <v>9</v>
       </c>
-      <c r="L21" s="5" t="n">
+      <c r="L21" s="5">
         <v>10</v>
       </c>
-      <c r="M21" s="5" t="n">
+      <c r="M21" s="5">
         <v>11</v>
       </c>
-      <c r="N21" s="5" t="n">
+      <c r="N21" s="5">
         <v>12</v>
       </c>
-      <c r="O21" s="5" t="n">
+      <c r="O21" s="5">
         <v>13</v>
       </c>
-      <c r="P21" s="5" t="n">
+      <c r="P21" s="5">
         <v>14</v>
       </c>
-      <c r="Q21" s="5" t="n">
+      <c r="Q21" s="5">
         <v>15</v>
       </c>
-      <c r="R21" s="5" t="n">
+      <c r="R21" s="5">
         <v>16</v>
       </c>
-      <c r="S21" s="5" t="n">
+      <c r="S21" s="5">
         <v>17</v>
       </c>
-      <c r="T21" s="5" t="n">
+      <c r="T21" s="5">
         <v>18</v>
       </c>
-      <c r="U21" s="5" t="n">
+      <c r="U21" s="5">
         <v>19</v>
       </c>
-      <c r="V21" s="5" t="n">
+      <c r="V21" s="5">
         <v>18</v>
       </c>
-      <c r="W21" s="5" t="n">
+      <c r="W21" s="5">
         <v>19</v>
       </c>
-      <c r="X21" s="5" t="n">
+      <c r="X21" s="5">
         <v>20</v>
       </c>
-      <c r="Y21" s="5" t="n">
+      <c r="Y21" s="5">
         <v>21</v>
       </c>
-      <c r="Z21" s="5" t="n">
+      <c r="Z21" s="5">
         <v>22</v>
       </c>
-      <c r="AA21" s="5" t="n">
-        <v>23</v>
-      </c>
-      <c r="AB21" s="5" t="n">
+      <c r="AA21" s="5">
+        <v>23</v>
+      </c>
+      <c r="AB21" s="5">
         <v>24</v>
       </c>
-      <c r="AC21" s="5" t="n">
+      <c r="AC21" s="5">
         <v>25</v>
       </c>
-      <c r="AD21" s="5" t="n">
+      <c r="AD21" s="5">
         <v>26</v>
       </c>
       <c r="AE21" s="6" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B22" s="8" t="s">
         <v>62</v>
       </c>
@@ -1157,39 +1487,37 @@
         <v>23</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B24" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B25" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B26" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B27" s="12" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" spans="1:31" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="B30" s="3" t="n">
+      <c r="B30" s="3">
         <v>0</v>
       </c>
       <c r="C30" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="G30" s="3" t="n">
+      <c r="G30" s="3">
         <v>1</v>
       </c>
       <c r="H30" s="6" t="s">
@@ -1199,8 +1527,8 @@
         <v>65</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="3" t="n">
+    <row r="31" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A31" s="3">
         <v>0</v>
       </c>
       <c r="B31" s="1" t="s">
@@ -1209,7 +1537,7 @@
       <c r="E31" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="F31" s="3" t="n">
+      <c r="F31" s="3">
         <v>0</v>
       </c>
       <c r="G31" s="1" t="s">
@@ -1219,8 +1547,8 @@
         <v>23</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="5" t="n">
+    <row r="32" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A32" s="5">
         <v>1</v>
       </c>
       <c r="B32" s="1" t="s">
@@ -1229,7 +1557,7 @@
       <c r="E32" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="F32" s="5" t="n">
+      <c r="F32" s="5">
         <v>1</v>
       </c>
       <c r="G32" s="1" t="s">
@@ -1239,8 +1567,8 @@
         <v>23</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="5" t="n">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" s="5">
         <v>2</v>
       </c>
       <c r="B33" s="1" t="s">
@@ -1249,7 +1577,7 @@
       <c r="E33" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="F33" s="5" t="n">
+      <c r="F33" s="5">
         <v>2</v>
       </c>
       <c r="G33" s="1" t="s">
@@ -1259,8 +1587,8 @@
         <v>23</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="5" t="n">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" s="5">
         <v>3</v>
       </c>
       <c r="B34" s="1" t="s">
@@ -1269,7 +1597,7 @@
       <c r="E34" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="F34" s="5" t="n">
+      <c r="F34" s="5">
         <v>3</v>
       </c>
       <c r="G34" s="1" t="s">
@@ -1279,8 +1607,8 @@
         <v>23</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="5" t="n">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35" s="5">
         <v>4</v>
       </c>
       <c r="B35" s="1" t="s">
@@ -1289,7 +1617,7 @@
       <c r="E35" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="F35" s="5" t="n">
+      <c r="F35" s="5">
         <v>4</v>
       </c>
       <c r="G35" s="1" t="s">
@@ -1299,7 +1627,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
         <v>2</v>
       </c>
@@ -1313,7 +1641,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="9" t="s">
         <v>65</v>
       </c>
@@ -1321,33 +1649,33 @@
         <v>65</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B38" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B39" s="1" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B40" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B41" s="12" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="10" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="3" t="n">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A46" s="3">
         <v>0</v>
       </c>
       <c r="B46" s="1" t="s">
@@ -1357,8 +1685,8 @@
         <v>23</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="5" t="n">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A47" s="5">
         <v>1</v>
       </c>
       <c r="B47" s="1" t="s">
@@ -1368,8 +1696,8 @@
         <v>23</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="5" t="n">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A48" s="5">
         <v>2</v>
       </c>
       <c r="B48" s="1" t="s">
@@ -1379,8 +1707,8 @@
         <v>23</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="5" t="n">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="5">
         <v>3</v>
       </c>
       <c r="B49" s="1" t="s">
@@ -1390,8 +1718,8 @@
         <v>23</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="5" t="n">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="5">
         <v>4</v>
       </c>
       <c r="B50" s="1" t="s">
@@ -1401,32 +1729,32 @@
         <v>23</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="6" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B53" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B54" s="12" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B55" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B56" s="12" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="10" t="s">
         <v>79</v>
       </c>
@@ -1446,50 +1774,50 @@
         <v>56</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B60" s="8" t="s">
         <v>84</v>
       </c>
       <c r="C60" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="D60" s="8" t="n">
+      <c r="D60" s="8">
         <v>1</v>
       </c>
-      <c r="E60" s="8" t="n">
+      <c r="E60" s="8">
         <v>20</v>
       </c>
       <c r="F60" s="9" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B63" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B64" s="1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B65" s="1" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B66" s="12" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A69" s="10" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="3" t="n">
+    <row r="70" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A70" s="3">
         <v>0</v>
       </c>
       <c r="B70" s="1" t="s">
@@ -1499,8 +1827,8 @@
         <v>23</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="5" t="n">
+    <row r="71" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A71" s="5">
         <v>1</v>
       </c>
       <c r="B71" s="1" t="s">
@@ -1510,8 +1838,8 @@
         <v>23</v>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="5" t="n">
+    <row r="72" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A72" s="5">
         <v>2</v>
       </c>
       <c r="B72" s="1" t="s">
@@ -1521,8 +1849,8 @@
         <v>23</v>
       </c>
     </row>
-    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="5" t="n">
+    <row r="73" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A73" s="5">
         <v>3</v>
       </c>
       <c r="B73" s="1" t="s">
@@ -1532,8 +1860,8 @@
         <v>23</v>
       </c>
     </row>
-    <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="5" t="n">
+    <row r="74" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A74" s="5">
         <v>4</v>
       </c>
       <c r="B74" s="1" t="s">
@@ -1543,8 +1871,8 @@
         <v>23</v>
       </c>
     </row>
-    <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="13" t="n">
+    <row r="75" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A75" s="13">
         <v>5</v>
       </c>
       <c r="B75" s="1" t="s">
@@ -1554,8 +1882,8 @@
         <v>23</v>
       </c>
     </row>
-    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="13" t="n">
+    <row r="76" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A76" s="13">
         <v>6</v>
       </c>
       <c r="B76" s="1" t="s">
@@ -1574,8 +1902,8 @@
         <v>73</v>
       </c>
     </row>
-    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="13" t="n">
+    <row r="77" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A77" s="13">
         <v>7</v>
       </c>
       <c r="B77" s="1" t="s">
@@ -1592,8 +1920,8 @@
       </c>
       <c r="Q77" s="1"/>
     </row>
-    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="13" t="n">
+    <row r="78" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A78" s="13">
         <v>8</v>
       </c>
       <c r="B78" s="1" t="s">
@@ -1603,8 +1931,8 @@
         <v>23</v>
       </c>
     </row>
-    <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="13" t="n">
+    <row r="79" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A79" s="13">
         <v>9</v>
       </c>
       <c r="B79" s="1" t="s">
@@ -1614,8 +1942,8 @@
         <v>23</v>
       </c>
     </row>
-    <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="13" t="n">
+    <row r="80" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A80" s="13">
         <v>10</v>
       </c>
       <c r="B80" s="1" t="s">
@@ -1625,8 +1953,8 @@
         <v>23</v>
       </c>
     </row>
-    <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="13" t="n">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A81" s="13">
         <v>11</v>
       </c>
       <c r="B81" s="1" t="s">
@@ -1636,7 +1964,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A82" s="6" t="s">
         <v>2</v>
       </c>
@@ -1644,38 +1972,130 @@
         <v>73</v>
       </c>
     </row>
-    <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A83" s="9" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B84" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B85" s="1" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B86" s="1" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B87" s="12" t="s">
         <v>102</v>
       </c>
     </row>
+    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A89" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D89" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="E89" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="F89" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="G89" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="H89" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="I89" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="J89" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="K89" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="L89" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A90" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D90" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="E90" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="F90" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="G90" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="H90" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="I90" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="J90" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="K90" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="L90" s="9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B92" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B93" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B94" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B95" s="12" t="s">
+        <v>126</v>
+      </c>
+    </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>